<commit_message>
limpando linhas com valores nulos e criando histogramas para cada maquina (ocorrencia x tempo[min])
</commit_message>
<xml_diff>
--- a/rcmPython.xlsx
+++ b/rcmPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Desktop\tcc_python\python-RCM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0CB9A4BE-A4EB-4325-A06F-D7BCAAA13C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{59C15073-8691-4CF9-988E-034AB5B4013D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17494,7 +17494,7 @@
   <dimension ref="A1:P422"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J426" sqref="J426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>